<commit_message>
fixing serial parsing issue
</commit_message>
<xml_diff>
--- a/Arduino-Bluetooth/data.xlsx
+++ b/Arduino-Bluetooth/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,42 +478,126 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0.36025617042292246</t>
+          <t>0.14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.36025617042292246</t>
+          <t>-0.02</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.36025617042292246</t>
+          <t>-0.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>05-Jan-2023 11:44:19</t>
+          <t>16-Jan-2023 23:04:07</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.36025617042292246</t>
+          <t>24.47</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.36025617042292246</t>
+          <t>-0.02</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.36025617042292246</t>
+          <t>-0.47</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>05-Jan-2023 11:44:19</t>
+          <t>16-Jan-2023 23:04:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>-0.03</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>-0.00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>16-Jan-2023 23:05:08</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>24.47</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-0.01</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-0.43999999999999995</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>16-Jan-2023 23:05:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>-0.02</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>-0.00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>16-Jan-2023 23:06:08</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>24.47</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>-0.02</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>-0.54</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>16-Jan-2023 23:06:08</t>
         </is>
       </c>
     </row>

</xml_diff>